<commit_message>
Add jumpers to schematic, BOM, drawing
</commit_message>
<xml_diff>
--- a/Source/Project Outputs for RUMBA32/RUMBA32_v1_0D_BOM.xlsx
+++ b/Source/Project Outputs for RUMBA32/RUMBA32_v1_0D_BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5408CD18-5674-4B30-92BD-F8479A5A84C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{255EB035-FCC0-448C-9EC9-2F19BED62A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105" xr2:uid="{1E4D46F0-58E1-4CFC-8A7B-76B211F9C8F8}"/>
+    <workbookView xWindow="1035" yWindow="1035" windowWidth="4110" windowHeight="10725" xr2:uid="{999C1F67-5990-464F-A3B6-045584E272FA}"/>
   </bookViews>
   <sheets>
     <sheet name="RUMBA32_v1_0D_BOM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="249">
   <si>
     <t>Designator</t>
   </si>
@@ -79,6 +79,27 @@
     <t>785-1689-1-ND</t>
   </si>
   <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>2.54mm .1" PCB Jumper, Green</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Installed as per drawing, approved sub OK</t>
+  </si>
+  <si>
+    <t>Sullins</t>
+  </si>
+  <si>
+    <t>QPC02SXGN-RC</t>
+  </si>
+  <si>
+    <t>S9337-ND</t>
+  </si>
+  <si>
     <t>U6</t>
   </si>
   <si>
@@ -250,7 +271,7 @@
     <t>Panasonic</t>
   </si>
   <si>
-    <t>EEE-FT1V101AP</t>
+    <t>EEEFT1V101AP</t>
   </si>
   <si>
     <t>PCE5016CT-ND</t>
@@ -439,6 +460,15 @@
     <t>Header 7X2</t>
   </si>
   <si>
+    <t>E0_0, E0_1, E1_0, E1_1, E2_0, E2_1, X_0, X_1, Y_0, Y_1, Z_0, Z_1</t>
+  </si>
+  <si>
+    <t>Header, 8-Pin, Female</t>
+  </si>
+  <si>
+    <t>Header 8</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
@@ -529,7 +559,7 @@
     <t>BUK9Y14-40B</t>
   </si>
   <si>
-    <t>NXP Semiconductors</t>
+    <t>Nexperia USA</t>
   </si>
   <si>
     <t>BUK9Y14-40B,115</t>
@@ -715,7 +745,7 @@
     <t>Phoenix Contact</t>
   </si>
   <si>
-    <t>1751264</t>
+    <t>MKDS1/4-3,5</t>
   </si>
   <si>
     <t>277-5744-ND</t>
@@ -727,7 +757,7 @@
     <t>3.5mm 2-Way</t>
   </si>
   <si>
-    <t>1751248</t>
+    <t>MKDS1/2-3,5</t>
   </si>
   <si>
     <t>277-5719-ND</t>
@@ -1136,8 +1166,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C299EFE-496D-4885-A902-C467EEE74A60}">
-  <dimension ref="A1:J46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E339CD-834C-4C1C-A16D-0EDC58A5DDAB}">
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1233,33 +1263,33 @@
         <v>11</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -1271,27 +1301,27 @@
         <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -1303,27 +1333,27 @@
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1335,39 +1365,39 @@
         <v>11</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>40</v>
@@ -1390,13 +1420,13 @@
         <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>46</v>
@@ -1416,147 +1446,147 @@
         <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="3">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10" s="3">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="E12" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E13" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>73</v>
@@ -1582,48 +1612,48 @@
         <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="E15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>86</v>
@@ -1640,214 +1670,214 @@
         <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E16" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E17" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="3">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>11</v>
@@ -1861,25 +1891,25 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="3">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>11</v>
@@ -1893,25 +1923,25 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="3">
-        <v>10</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>11</v>
@@ -1925,25 +1955,25 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>11</v>
@@ -1957,25 +1987,25 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>11</v>
@@ -1989,25 +2019,25 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>11</v>
@@ -2021,34 +2051,34 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>143</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2056,86 +2086,86 @@
         <v>144</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>146</v>
+        <v>11</v>
       </c>
       <c r="E29" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>147</v>
+        <v>11</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>148</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="3">
-        <v>11</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>157</v>
@@ -2155,36 +2185,36 @@
         <v>160</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>166</v>
@@ -2193,33 +2223,33 @@
         <v>11</v>
       </c>
       <c r="E33" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="G33" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="I33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>172</v>
+        <v>11</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>11</v>
@@ -2228,123 +2258,123 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="3">
+        <v>5</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="H35" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="I35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="E35" s="3">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="H36" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="I36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E36" s="3">
-        <v>10</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="H37" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E37" s="3">
-        <v>2</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H37" s="4" t="s">
+      <c r="I37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>195</v>
@@ -2353,13 +2383,13 @@
         <v>196</v>
       </c>
       <c r="E38" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>197</v>
@@ -2376,7 +2406,7 @@
         <v>199</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>200</v>
@@ -2388,10 +2418,10 @@
         <v>2</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>202</v>
@@ -2408,7 +2438,7 @@
         <v>204</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>205</v>
@@ -2420,74 +2450,74 @@
         <v>11</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G40" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H40" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="I40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="3">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="E41" s="3">
-        <v>13</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H41" s="4" t="s">
+      <c r="I41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="3">
+        <v>11</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="E42" s="3">
-        <v>6</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>218</v>
@@ -2504,7 +2534,7 @@
         <v>220</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>221</v>
@@ -2513,13 +2543,13 @@
         <v>222</v>
       </c>
       <c r="E43" s="3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>223</v>
@@ -2536,54 +2566,54 @@
         <v>225</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E44" s="3">
         <v>6</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G44" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="I44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J44" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E45" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>228</v>
+        <v>59</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>233</v>
@@ -2600,172 +2630,242 @@
         <v>235</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="3">
+        <v>6</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="3">
+      <c r="C47" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="3">
+        <v>5</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="3">
         <v>3</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J46" s="4" t="s">
+      <c r="F48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>238</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{7754A06B-A886-47CC-95CE-7237FD1CDFF5}"/>
-    <hyperlink ref="H2" r:id="rId2" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{87B110CA-DF83-485C-BD18-21E4B76A115C}"/>
-    <hyperlink ref="J2" r:id="rId3" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{DE6157E4-45DD-4199-A693-2CF417EC158E}"/>
-    <hyperlink ref="G3" r:id="rId4" tooltip="Component" display="'Diodes" xr:uid="{7DA98EDC-9501-485C-A0E9-4A5BF41FD961}"/>
-    <hyperlink ref="H3" r:id="rId5" tooltip="Manufacturer" display="'AP2112K-3.3TRG1" xr:uid="{F9CAD97D-A616-40B7-B909-C11A1DB3BEF4}"/>
-    <hyperlink ref="J3" r:id="rId6" tooltip="Supplier" display="'AP2112K-3.3TRG1DICT-ND" xr:uid="{0D01A3E4-0BFF-4666-AFB7-8F1A838E8585}"/>
-    <hyperlink ref="G4" r:id="rId7" tooltip="Component" display="'STMicroelectronics" xr:uid="{81571004-5AF3-4D1B-AD26-93273E8421A7}"/>
-    <hyperlink ref="H4" r:id="rId8" tooltip="Manufacturer" display="'STM32F446VET6" xr:uid="{806BEFB2-543E-452E-88C0-592D82D4A9AE}"/>
-    <hyperlink ref="J4" r:id="rId9" tooltip="Supplier" display="'497-15375-ND" xr:uid="{C7632DB1-0F19-4FF2-AD69-F36A1DCFA8AB}"/>
-    <hyperlink ref="G5" r:id="rId10" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{A77C0F14-B29F-4DD0-813C-1877BC1A0D60}"/>
-    <hyperlink ref="H5" r:id="rId11" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{B4F7E855-00F7-4E33-97EF-3A59CB574F42}"/>
-    <hyperlink ref="J5" r:id="rId12" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{8F3461E5-2196-4EF5-9D65-5F029349D763}"/>
-    <hyperlink ref="G6" r:id="rId13" tooltip="Component" display="'Diodes" xr:uid="{3D0C119B-9066-4F7E-8BEA-5EB80DDF822E}"/>
-    <hyperlink ref="H6" r:id="rId14" tooltip="Manufacturer" display="'74LVC1G17SE-7" xr:uid="{E177ED95-EB45-4D58-90B2-CF949A1C4462}"/>
-    <hyperlink ref="J6" r:id="rId15" tooltip="Supplier" display="'74LVC1G17SE-7CT-ND" xr:uid="{24EF2817-330B-4179-936C-17DF221457B7}"/>
-    <hyperlink ref="G7" r:id="rId16" tooltip="Component" display="'APEM" xr:uid="{147B6F2F-2D3E-4875-B285-8442FD0A6178}"/>
-    <hyperlink ref="H7" r:id="rId17" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{A5E79D27-1860-46A0-B7E7-343590D4B55A}"/>
-    <hyperlink ref="J7" r:id="rId18" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{152DE351-12A2-4085-A683-4259F2CA9E66}"/>
-    <hyperlink ref="G8" r:id="rId19" tooltip="Component" display="'TDK" xr:uid="{A1081C98-1B31-4CB7-8B0E-CE7DF4683117}"/>
-    <hyperlink ref="H8" r:id="rId20" tooltip="Manufacturer" display="'C1608X7R1C105K080AC" xr:uid="{6A8F6CAE-07E7-46C8-8753-A95EB6DCEE29}"/>
-    <hyperlink ref="J8" r:id="rId21" tooltip="Supplier" display="'445-1604-1-ND" xr:uid="{A53DF031-77A6-4C7D-90BE-F45090108774}"/>
-    <hyperlink ref="G9" r:id="rId22" tooltip="Component" display="'Yageo" xr:uid="{4ED3A51E-C28F-447B-B109-C1EBD0E0DBF4}"/>
-    <hyperlink ref="H9" r:id="rId23" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{796219B9-AC37-4683-AB54-67775A67CCCE}"/>
-    <hyperlink ref="J9" r:id="rId24" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{1043EEBA-D658-491E-AB59-D400CEA4996B}"/>
-    <hyperlink ref="G10" r:id="rId25" tooltip="Component" display="'TDK" xr:uid="{663674E2-C748-495E-842A-01577BA73B2E}"/>
-    <hyperlink ref="H10" r:id="rId26" tooltip="Manufacturer" display="'C1608X7R1C105K080AC" xr:uid="{3B39B707-1CCC-4F75-84D2-B5943D504307}"/>
-    <hyperlink ref="J10" r:id="rId27" tooltip="Supplier" display="'445-1604-1-ND" xr:uid="{4737554F-2D3C-4A34-8C0F-A98CAE3B6E07}"/>
-    <hyperlink ref="G11" r:id="rId28" tooltip="Component" display="'Samsung" xr:uid="{0B7EE49B-5690-400D-AF78-F7286BC3FCB3}"/>
-    <hyperlink ref="H11" r:id="rId29" tooltip="Manufacturer" display="'CL21A106KQFNNNG" xr:uid="{7A0DBA31-0322-4406-AFD2-250A97247F2A}"/>
-    <hyperlink ref="J11" r:id="rId30" tooltip="Supplier" display="'1276-6457-1-ND" xr:uid="{84BE5D5F-A95E-4E28-A772-627CF6710DCA}"/>
-    <hyperlink ref="G12" r:id="rId31" tooltip="Component" display="'Murata" xr:uid="{8FAEE21C-2204-4960-BCFD-A3C8129D0160}"/>
-    <hyperlink ref="H12" r:id="rId32" tooltip="Manufacturer" display="'GRM32ER71H475KA88L" xr:uid="{6EA954C7-8FA4-4FF7-B615-24685AA4D1EB}"/>
-    <hyperlink ref="J12" r:id="rId33" tooltip="Supplier" display="'490-1864-1-ND" xr:uid="{1ACF1E47-4005-418B-AC04-877803CE11D3}"/>
-    <hyperlink ref="G13" r:id="rId34" tooltip="Component" display="'Panasonic" xr:uid="{AB5405AB-2A32-4658-892D-CF7D6DD2B470}"/>
-    <hyperlink ref="H13" r:id="rId35" tooltip="Manufacturer" display="'EEE-FT1V101AP" xr:uid="{DB153776-960E-46C3-A022-C23982994F2D}"/>
-    <hyperlink ref="J13" r:id="rId36" tooltip="Supplier" display="'PCE5016CT-ND" xr:uid="{FD7C5421-33D2-4A41-9F40-AD36AB14D706}"/>
-    <hyperlink ref="G14" r:id="rId37" tooltip="Component" display="'Murata" xr:uid="{90E2A490-A93D-4E8E-97E7-70FB88094A63}"/>
-    <hyperlink ref="H14" r:id="rId38" tooltip="Manufacturer" display="'CSTCE12M0G55-R0" xr:uid="{088B0EAE-2E18-4176-89E6-4B5700705582}"/>
-    <hyperlink ref="J14" r:id="rId39" tooltip="Supplier" display="'490-1197-1-ND" xr:uid="{4D4B8CCB-78F5-4ADC-B689-CC3772689839}"/>
-    <hyperlink ref="G15" r:id="rId40" tooltip="Component" display="'General Instruments" xr:uid="{BD000428-C6C4-43B3-ADDD-37E5545336EA}"/>
-    <hyperlink ref="H15" r:id="rId41" tooltip="Manufacturer" display="'SSB44-E3/52T" xr:uid="{3219A558-18E3-4856-98E9-2C21796F73AE}"/>
-    <hyperlink ref="J15" r:id="rId42" tooltip="Supplier" display="'SSB44-E3/52TGICT-ND" xr:uid="{2FDA3E72-31B2-45B2-A5F4-B57A7E8D1651}"/>
-    <hyperlink ref="G16" r:id="rId43" tooltip="Component" display="'ON Semiconductor / Fairchild" xr:uid="{F789A4E8-F32B-4F22-8AFE-444ABAB1D740}"/>
-    <hyperlink ref="H16" r:id="rId44" tooltip="Manufacturer" display="'SS24FL" xr:uid="{295D2074-1CF8-4C0C-B78E-5253610E324A}"/>
-    <hyperlink ref="J16" r:id="rId45" tooltip="Supplier" display="'SS24FLCT-ND" xr:uid="{92EA4275-9A20-41AF-9113-9AF011A16175}"/>
-    <hyperlink ref="G17" r:id="rId46" tooltip="Component" display="'Diodes" xr:uid="{3C359F3A-E167-4081-98AD-75203B5385A4}"/>
-    <hyperlink ref="H17" r:id="rId47" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{BBE8C9EB-947A-4848-A5C1-0266642BD7FC}"/>
-    <hyperlink ref="J17" r:id="rId48" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{8DE04F34-701C-413E-940A-8FB3C33FCE95}"/>
-    <hyperlink ref="G18" r:id="rId49" tooltip="Component" display="'STMicroelectronics" xr:uid="{3376E2FD-8E81-4994-AA2B-DD327C0688F0}"/>
-    <hyperlink ref="H18" r:id="rId50" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{DA3F6694-14D2-4109-A4A3-AA3BEB1E43A7}"/>
-    <hyperlink ref="J18" r:id="rId51" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{3DA45DCB-2CD5-42DC-BF92-19D4413691B8}"/>
-    <hyperlink ref="G19" r:id="rId52" tooltip="Component" display="'Murata" xr:uid="{38B8551F-09A9-4A94-B4B0-905F58AEEA5F}"/>
-    <hyperlink ref="H19" r:id="rId53" tooltip="Manufacturer" display="'BLM18PG-121SN1D" xr:uid="{D4793293-9C03-44CB-BE32-3DF856D6EF46}"/>
-    <hyperlink ref="J19" r:id="rId54" tooltip="Supplier" display="'490-1037-1-ND" xr:uid="{C48D2A36-6AB8-4537-9814-FA8793DAF8ED}"/>
-    <hyperlink ref="G20" r:id="rId55" tooltip="Component" display="'Memory Protection Devices" xr:uid="{29AA2DAF-FFF1-4889-A837-F7D8641E47C3}"/>
-    <hyperlink ref="H20" r:id="rId56" tooltip="Manufacturer" display="'BK-6013" xr:uid="{BB6D67A4-147C-475A-A555-80048A02E49B}"/>
-    <hyperlink ref="J20" r:id="rId57" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{A4F5D28F-BA36-4E7D-AD25-7B954D95F154}"/>
-    <hyperlink ref="G21" tooltip="Component" display="'Generic Header" xr:uid="{0383FD7D-BB25-4972-B16A-1901BE11166A}"/>
-    <hyperlink ref="H21" tooltip="Manufacturer" display="'" xr:uid="{B78A32BC-4624-4BC1-ABFE-D6055A3115FA}"/>
-    <hyperlink ref="J21" tooltip="Supplier" display="'" xr:uid="{0912A844-EC4F-44CD-8172-7B0EE005D816}"/>
-    <hyperlink ref="G22" tooltip="Component" display="'Generic Header" xr:uid="{4488FDFC-D9F0-4936-AD3A-F73CED78F7F0}"/>
-    <hyperlink ref="H22" tooltip="Manufacturer" display="'" xr:uid="{CC53514C-5CD6-4AC4-8A6E-79A415E0253E}"/>
-    <hyperlink ref="J22" tooltip="Supplier" display="'" xr:uid="{EA1186D7-2103-48EB-A54F-2EBA4DE81553}"/>
-    <hyperlink ref="G23" tooltip="Component" display="'Generic Header" xr:uid="{5904AB25-41F2-4B8D-947E-15C49A8AE508}"/>
-    <hyperlink ref="H23" tooltip="Manufacturer" display="'" xr:uid="{146EC5C3-427C-4D5B-A04B-9B14B2BD9573}"/>
-    <hyperlink ref="J23" tooltip="Supplier" display="'" xr:uid="{F9EEAA79-81DD-4D55-B2DA-AD5E09CDEF91}"/>
-    <hyperlink ref="G24" tooltip="Component" display="'Generic Header" xr:uid="{56FEA2B1-F516-47BA-AB6D-2C61DC671E41}"/>
-    <hyperlink ref="H24" tooltip="Manufacturer" display="'" xr:uid="{63512C07-7B67-44E6-8ECA-55F7F21AF6C1}"/>
-    <hyperlink ref="J24" tooltip="Supplier" display="'" xr:uid="{CEBC4C4D-E0E6-4E4C-AD35-2DFDD312C899}"/>
-    <hyperlink ref="G25" tooltip="Component" display="'Generic Header" xr:uid="{3B764E1D-6CF0-4566-A4FD-DBBE79988C4B}"/>
-    <hyperlink ref="H25" tooltip="Manufacturer" display="'" xr:uid="{63DD00AD-AF2F-45C8-B84B-1337A484E2A0}"/>
-    <hyperlink ref="J25" tooltip="Supplier" display="'" xr:uid="{31531B45-C294-4568-AE58-5BA6B89EACAE}"/>
-    <hyperlink ref="G26" tooltip="Component" display="'Generic Header" xr:uid="{209AC512-E5B9-4822-882E-9D62B162F39D}"/>
-    <hyperlink ref="H26" tooltip="Manufacturer" display="'" xr:uid="{E5C060C9-1142-465E-9A26-F9BF100B8904}"/>
-    <hyperlink ref="J26" tooltip="Supplier" display="'" xr:uid="{3940C85B-817A-4ECA-830A-A2F36A4882ED}"/>
-    <hyperlink ref="G27" tooltip="Component" display="'Generic Header" xr:uid="{E552AE22-02B3-4EF4-B222-FDF9F2569B5A}"/>
-    <hyperlink ref="H27" tooltip="Manufacturer" display="'" xr:uid="{3330E718-C177-4337-A45B-A6B39A731044}"/>
-    <hyperlink ref="J27" tooltip="Supplier" display="'" xr:uid="{1705C967-024D-4B81-93A7-16D3368C82E9}"/>
-    <hyperlink ref="G28" r:id="rId58" tooltip="Component" display="'Bourns" xr:uid="{F7A000E2-6D6C-4943-B81A-B90588558D6B}"/>
-    <hyperlink ref="H28" r:id="rId59" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{AC97E83E-0C64-4C3B-A5D0-8E1624B41F37}"/>
-    <hyperlink ref="J28" r:id="rId60" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{C8F67FC5-609F-4860-A70A-9F5DFD5000AC}"/>
-    <hyperlink ref="G29" r:id="rId61" tooltip="Component" display="'Bourns" xr:uid="{86BD5977-404F-4F91-9526-7304E09719CF}"/>
-    <hyperlink ref="H29" r:id="rId62" tooltip="Manufacturer" display="'SRN6045TA-4R7M" xr:uid="{7974563A-A8B9-4A9F-AA83-A0A7EAEA8DF0}"/>
-    <hyperlink ref="J29" r:id="rId63" tooltip="Supplier" display="'SRN6045TA-4R7MCT-ND" xr:uid="{C5C9F743-383B-4B78-88B5-B5C46BBBFAA4}"/>
-    <hyperlink ref="G30" r:id="rId64" tooltip="Component" display="'Vishay Lite-On" xr:uid="{7B6C1221-5121-4E76-B357-A5933FFBB6E7}"/>
-    <hyperlink ref="H30" r:id="rId65" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{BCD1F9A3-9151-4E3E-BEF4-23502CDE11D6}"/>
-    <hyperlink ref="J30" r:id="rId66" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{ACF82566-AA3C-44BE-8D33-F4885C344AF8}"/>
-    <hyperlink ref="G31" r:id="rId67" tooltip="Component" display="'Vishay Lite-On" xr:uid="{4730E9B9-5169-4A34-87DC-C7DBB77DC5F6}"/>
-    <hyperlink ref="H31" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{9099B79B-C9D2-43A5-8D7A-2C3FE2FCEE11}"/>
-    <hyperlink ref="J31" r:id="rId69" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{0CCD54CB-A8FA-4D0E-9205-481432CF6B43}"/>
-    <hyperlink ref="G32" r:id="rId70" tooltip="Component" display="'Molex" xr:uid="{00AEC4C0-ECF3-4490-992B-76C4EE7234E2}"/>
-    <hyperlink ref="H32" r:id="rId71" tooltip="Manufacturer" display="'105017-0001" xr:uid="{3F50DF3D-30C0-4474-819B-8B2D2156DFCB}"/>
-    <hyperlink ref="J32" r:id="rId72" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{619FB806-762A-410E-9103-2D97B1CCE0E5}"/>
-    <hyperlink ref="G33" r:id="rId73" tooltip="Component" display="'NXP Semiconductors" xr:uid="{38F45E77-2C2F-4929-BACD-936766FFD22D}"/>
-    <hyperlink ref="H33" r:id="rId74" tooltip="Manufacturer" display="'BUK9Y14-40B,115" xr:uid="{1B0F8451-D09B-43C6-AFA0-36996B81B3EA}"/>
-    <hyperlink ref="J33" r:id="rId75" tooltip="Supplier" display="'1727-4940-1-ND" xr:uid="{173D7ACF-13F7-49A5-89F3-D9FD72CC2347}"/>
-    <hyperlink ref="G34" r:id="rId76" tooltip="Component" display="'Vishay Siliconix" xr:uid="{CAF39F5A-7D9A-46F5-A2C2-CA563BD10E79}"/>
-    <hyperlink ref="H34" r:id="rId77" tooltip="Manufacturer" display="'SISS10DN-T1-GE3" xr:uid="{C8107C03-E39C-4408-829D-3DD8F177E69C}"/>
-    <hyperlink ref="J34" r:id="rId78" tooltip="Supplier" display="'SISS10DN-T1-GE3CT-ND" xr:uid="{307BA1B0-2426-4BD0-BEE7-B5259B82522B}"/>
-    <hyperlink ref="G35" r:id="rId79" tooltip="Component" display="'Bel" xr:uid="{F35F30F1-36E8-4A67-B801-11B9E9BBC75C}"/>
-    <hyperlink ref="H35" r:id="rId80" tooltip="Manufacturer" display="'0ZCM0020FF2G" xr:uid="{47D84BA0-5934-44EA-BE01-903FBFD01C7C}"/>
-    <hyperlink ref="J35" r:id="rId81" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{84C02512-2975-4807-926B-45E51E39913B}"/>
-    <hyperlink ref="G36" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{FE1B2292-0750-4C8E-8D18-73F582FCC6E3}"/>
-    <hyperlink ref="H36" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{D14E450F-A7B7-4EA3-84BA-622BF4303D14}"/>
-    <hyperlink ref="J36" r:id="rId84" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{795B36C3-2C66-4C64-9CCF-69B8C3863CA5}"/>
-    <hyperlink ref="G37" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{1F7A2D7E-AFFA-4349-BAEB-C7B5C5EE4B23}"/>
-    <hyperlink ref="H37" r:id="rId86" tooltip="Manufacturer" display="'RC0603JR-072K2L" xr:uid="{923F9C1A-60AE-4BA5-AB0E-7E788C02D0CB}"/>
-    <hyperlink ref="J37" r:id="rId87" tooltip="Supplier" display="'311-2.2KGRCT-ND" xr:uid="{0C6ACD3E-9EA2-4793-9CC3-BE94F73D97CB}"/>
-    <hyperlink ref="G38" r:id="rId88" tooltip="Component" display="'Yageo" xr:uid="{595B6819-2E67-4A84-8868-6E5019083607}"/>
-    <hyperlink ref="H38" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{10E01C78-0A59-4752-917E-026183B44F22}"/>
-    <hyperlink ref="J38" r:id="rId90" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{348BB5EC-0DD9-4568-9DAA-54CE6DA8BE20}"/>
-    <hyperlink ref="G39" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{5DD9F9EF-5CE3-439A-99CA-774DC23C4677}"/>
-    <hyperlink ref="H39" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0754K9L" xr:uid="{9B6DCFE8-46FA-46A8-BB76-1961B63A2334}"/>
-    <hyperlink ref="J39" r:id="rId93" tooltip="Supplier" display="'311-54.9KHRCT-ND" xr:uid="{CD40FD53-73A3-4A29-9E32-579115A86034}"/>
-    <hyperlink ref="G40" r:id="rId94" tooltip="Component" display="'Yageo Phycomp" xr:uid="{FDCA24D5-BBA5-49B9-8B1A-3942F8535DE1}"/>
-    <hyperlink ref="H40" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{452E32C3-A783-4686-85CA-676A8B047600}"/>
-    <hyperlink ref="J40" r:id="rId96" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{DDA25DB0-9537-4B2E-B031-C6EE879BB472}"/>
-    <hyperlink ref="G41" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{0ABF129E-A43D-41D2-AFFF-3B47B1532C1B}"/>
-    <hyperlink ref="H41" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{3B74536B-E05B-46B3-874A-0286D08B0134}"/>
-    <hyperlink ref="J41" r:id="rId99" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{BE0A2D21-D597-4F3D-9E03-E4C9D77433CA}"/>
-    <hyperlink ref="G42" r:id="rId100" tooltip="Component" display="'Yageo Phycomp" xr:uid="{0431065F-DC75-432A-9C98-157B366D0934}"/>
-    <hyperlink ref="H42" r:id="rId101" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{6CEC50EE-CDBE-41C3-8242-AF798FB3AFB6}"/>
-    <hyperlink ref="J42" r:id="rId102" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{3F439DF0-C976-47DD-B306-3F3A3375ACA6}"/>
-    <hyperlink ref="G43" r:id="rId103" tooltip="Component" display="'Yageo" xr:uid="{57666B35-2558-4A7C-A0C1-017B2EC0ACD1}"/>
-    <hyperlink ref="H43" r:id="rId104" tooltip="Manufacturer" display="'RC0603FR-07140KL" xr:uid="{D3CF101C-8F82-4EFB-8EDE-7E3E6BC98A1E}"/>
-    <hyperlink ref="J43" r:id="rId105" tooltip="Supplier" display="'311-140KHRCT-ND" xr:uid="{322F9F6C-7C1C-4894-B1F1-22830F88458A}"/>
-    <hyperlink ref="G44" r:id="rId106" tooltip="Component" display="'Phoenix Contact" xr:uid="{1CD59CEB-0CBD-4F9B-8A06-2A140E109F4C}"/>
-    <hyperlink ref="H44" r:id="rId107" tooltip="Manufacturer" display="'1751264" xr:uid="{EDEA4FA3-FE7B-4481-B7EB-AFA1E4AA9C1F}"/>
-    <hyperlink ref="J44" r:id="rId108" tooltip="Supplier" display="'277-5744-ND" xr:uid="{0034E6F8-837A-4FD5-A69F-3CE548F063B9}"/>
-    <hyperlink ref="G45" r:id="rId109" tooltip="Component" display="'Phoenix Contact" xr:uid="{21D7C27C-FE74-43B8-9CD9-04DD157374F3}"/>
-    <hyperlink ref="H45" r:id="rId110" tooltip="Manufacturer" display="'1751248" xr:uid="{2CF4C351-33BD-4552-8474-9CD8C12DB114}"/>
-    <hyperlink ref="J45" r:id="rId111" tooltip="Supplier" display="'277-5719-ND" xr:uid="{2600B56A-4564-40BF-95DC-5D225EB55997}"/>
-    <hyperlink ref="G46" r:id="rId112" tooltip="Component" display="'Phoenix Contact" xr:uid="{FBC9E2D1-5F41-402B-B1D3-795841D11FD5}"/>
-    <hyperlink ref="H46" r:id="rId113" tooltip="Manufacturer" display="'1935776" xr:uid="{8DE09A71-238C-4B44-8D6A-CA4B89DF7917}"/>
-    <hyperlink ref="J46" r:id="rId114" tooltip="Supplier" display="'277-6405-ND" xr:uid="{79F8C930-0424-4197-91F2-3D9783E22B94}"/>
+    <hyperlink ref="G2" r:id="rId1" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{FDFF70C6-22FD-4C13-81BD-F6847BDA953D}"/>
+    <hyperlink ref="H2" r:id="rId2" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{33400E7B-E601-413B-9559-15A39977FC85}"/>
+    <hyperlink ref="J2" r:id="rId3" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{677578C8-A45A-4E89-AEC5-672989547972}"/>
+    <hyperlink ref="G3" r:id="rId4" tooltip="Component" display="'Sullins" xr:uid="{EDB7C494-6ADD-40DC-85AA-5FA556F3DBFC}"/>
+    <hyperlink ref="H3" r:id="rId5" tooltip="Manufacturer" display="'QPC02SXGN-RC" xr:uid="{E9E35BAA-5AB9-4A38-86E2-4D7630C91007}"/>
+    <hyperlink ref="J3" r:id="rId6" tooltip="Supplier" display="'S9337-ND" xr:uid="{B56A7BE8-A800-4291-88C9-9C4469E6F044}"/>
+    <hyperlink ref="G4" r:id="rId7" tooltip="Component" display="'Diodes" xr:uid="{2EEAB141-D698-4A97-9924-663A5FD2E04F}"/>
+    <hyperlink ref="H4" r:id="rId8" tooltip="Manufacturer" display="'AP2112K-3.3TRG1" xr:uid="{09574C23-5A45-494A-B977-99FEE5DAC92E}"/>
+    <hyperlink ref="J4" r:id="rId9" tooltip="Supplier" display="'AP2112K-3.3TRG1DICT-ND" xr:uid="{7E9906BE-A085-4DFF-9955-CAE558715388}"/>
+    <hyperlink ref="G5" r:id="rId10" tooltip="Component" display="'STMicroelectronics" xr:uid="{51462FAB-2A67-481A-944F-03E0F638EA6E}"/>
+    <hyperlink ref="H5" r:id="rId11" tooltip="Manufacturer" display="'STM32F446VET6" xr:uid="{B4E921DD-78F9-4DC6-B315-309D4C73AE8B}"/>
+    <hyperlink ref="J5" r:id="rId12" tooltip="Supplier" display="'497-15375-ND" xr:uid="{172E9B85-1E1F-4A7C-B7A4-199D7996F93B}"/>
+    <hyperlink ref="G6" r:id="rId13" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{D9416DC3-B77A-495D-BC2E-9FF6BE06C843}"/>
+    <hyperlink ref="H6" r:id="rId14" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{EC064FB7-DF51-4C60-8BBA-35AB6B009D3E}"/>
+    <hyperlink ref="J6" r:id="rId15" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{372DEFB2-B22B-422A-BC34-154723EF198A}"/>
+    <hyperlink ref="G7" r:id="rId16" tooltip="Component" display="'Diodes" xr:uid="{E6E94D93-C408-4BEB-97C5-30D6C8356BD5}"/>
+    <hyperlink ref="H7" r:id="rId17" tooltip="Manufacturer" display="'74LVC1G17SE-7" xr:uid="{DFB8A851-8CDB-4BCE-B61A-D65F2B140B42}"/>
+    <hyperlink ref="J7" r:id="rId18" tooltip="Supplier" display="'74LVC1G17SE-7CT-ND" xr:uid="{0CD63918-C2ED-4190-959B-039B5DA117C0}"/>
+    <hyperlink ref="G8" r:id="rId19" tooltip="Component" display="'APEM" xr:uid="{525AA35E-5AEC-4EFF-9469-29F6879EFAF8}"/>
+    <hyperlink ref="H8" r:id="rId20" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{752E4203-2B82-483C-BA46-65E5D1899D9B}"/>
+    <hyperlink ref="J8" r:id="rId21" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{E8AD966E-D6BF-4A3B-924F-0AA5403D6E2A}"/>
+    <hyperlink ref="G9" r:id="rId22" tooltip="Component" display="'TDK" xr:uid="{4D71B14A-EA7D-43BA-AE58-29EB8E1FC4AC}"/>
+    <hyperlink ref="H9" r:id="rId23" tooltip="Manufacturer" display="'C1608X7R1C105K080AC" xr:uid="{406DE07A-4C24-4331-BFBC-6F04FB96625D}"/>
+    <hyperlink ref="J9" r:id="rId24" tooltip="Supplier" display="'445-1604-1-ND" xr:uid="{D7DB5473-E3BA-431D-A43B-54F68ADFB2A6}"/>
+    <hyperlink ref="G10" r:id="rId25" tooltip="Component" display="'Yageo" xr:uid="{CD158F46-5A53-4599-AEF8-71AB0B6DC785}"/>
+    <hyperlink ref="H10" r:id="rId26" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{3DB3966D-275E-43CD-9934-CFBF06988BA9}"/>
+    <hyperlink ref="J10" r:id="rId27" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{1182805A-5466-4639-B523-AABBFD57D667}"/>
+    <hyperlink ref="G11" r:id="rId28" tooltip="Component" display="'TDK" xr:uid="{7F1519DF-70F9-404F-96FF-EE28121C20C4}"/>
+    <hyperlink ref="H11" r:id="rId29" tooltip="Manufacturer" display="'C1608X7R1C105K080AC" xr:uid="{72CA5945-5FF8-40A0-AA93-AC82EFCF6FA0}"/>
+    <hyperlink ref="J11" r:id="rId30" tooltip="Supplier" display="'445-1604-1-ND" xr:uid="{825F7DA8-C35B-449D-9D91-06B8C9D5CCBA}"/>
+    <hyperlink ref="G12" r:id="rId31" tooltip="Component" display="'Samsung" xr:uid="{126774D3-7D49-4BE7-941A-76ABE7487F3E}"/>
+    <hyperlink ref="H12" r:id="rId32" tooltip="Manufacturer" display="'CL21A106KQFNNNG" xr:uid="{2E28700B-DAAD-4849-8124-EEA6F4C9178B}"/>
+    <hyperlink ref="J12" r:id="rId33" tooltip="Supplier" display="'1276-6457-1-ND" xr:uid="{AE68BBD1-87F9-41B5-AB90-2BD1DA2BE2E4}"/>
+    <hyperlink ref="G13" r:id="rId34" tooltip="Component" display="'Murata" xr:uid="{83A33889-7159-41EB-A66C-65B68E559497}"/>
+    <hyperlink ref="H13" r:id="rId35" tooltip="Manufacturer" display="'GRM32ER71H475KA88L" xr:uid="{5B4BBFB8-4943-4A7C-B454-01D66FFF8835}"/>
+    <hyperlink ref="J13" r:id="rId36" tooltip="Supplier" display="'490-1864-1-ND" xr:uid="{D1D2D63A-4DAB-49F6-8DCA-019C5BD8C519}"/>
+    <hyperlink ref="G14" r:id="rId37" tooltip="Component" display="'Panasonic" xr:uid="{4D51A039-72A8-4598-8027-97A6B91B9C39}"/>
+    <hyperlink ref="H14" r:id="rId38" tooltip="Manufacturer" display="'EEEFT1V101AP" xr:uid="{BF18AABA-7853-4BA0-84AD-31EAD07EA030}"/>
+    <hyperlink ref="J14" r:id="rId39" tooltip="Supplier" display="'PCE5016CT-ND" xr:uid="{C3EA5395-CC0E-4540-BA57-1CD74BE1ECBC}"/>
+    <hyperlink ref="G15" r:id="rId40" tooltip="Component" display="'Murata" xr:uid="{1066A65E-9FC9-49BA-B49D-C6D6D722EB70}"/>
+    <hyperlink ref="H15" r:id="rId41" tooltip="Manufacturer" display="'CSTCE12M0G55-R0" xr:uid="{04D0694A-F386-401F-8FF1-BF8EEA75090A}"/>
+    <hyperlink ref="J15" r:id="rId42" tooltip="Supplier" display="'490-1197-1-ND" xr:uid="{FE92C673-DBAC-4B1D-9C87-DB133B65E28B}"/>
+    <hyperlink ref="G16" r:id="rId43" tooltip="Component" display="'General Instruments" xr:uid="{54633E24-A445-457C-971F-BC6F4E416274}"/>
+    <hyperlink ref="H16" r:id="rId44" tooltip="Manufacturer" display="'SSB44-E3/52T" xr:uid="{63BFA57F-A791-4BAA-B7E0-94F30C2E37F0}"/>
+    <hyperlink ref="J16" r:id="rId45" tooltip="Supplier" display="'SSB44-E3/52TGICT-ND" xr:uid="{5DE7AC22-E7B7-4599-9F26-46B519141ADB}"/>
+    <hyperlink ref="G17" r:id="rId46" tooltip="Component" display="'ON Semiconductor / Fairchild" xr:uid="{E1B0405A-A89A-44E3-8BD7-F5EEF0E1F52C}"/>
+    <hyperlink ref="H17" r:id="rId47" tooltip="Manufacturer" display="'SS24FL" xr:uid="{F6FDFE44-6A37-4008-98B2-19D95502F617}"/>
+    <hyperlink ref="J17" r:id="rId48" tooltip="Supplier" display="'SS24FLCT-ND" xr:uid="{65814575-0615-45FF-B314-3985D118D90C}"/>
+    <hyperlink ref="G18" r:id="rId49" tooltip="Component" display="'Diodes" xr:uid="{FBA8E2CE-7A7A-4494-BCC7-A2CD3857988D}"/>
+    <hyperlink ref="H18" r:id="rId50" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{5CCF8047-9775-4575-982C-CD72069804B0}"/>
+    <hyperlink ref="J18" r:id="rId51" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{7C8BEFD9-99BC-42CC-BEB7-B2D430141F2B}"/>
+    <hyperlink ref="G19" r:id="rId52" tooltip="Component" display="'STMicroelectronics" xr:uid="{52C39956-454D-4022-A7DC-088A7CB75235}"/>
+    <hyperlink ref="H19" r:id="rId53" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{AF7398F3-431F-4A6D-B7C5-A5D428D2A7A3}"/>
+    <hyperlink ref="J19" r:id="rId54" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{02FCE4F4-2534-4F53-8905-ACE0B728D496}"/>
+    <hyperlink ref="G20" r:id="rId55" tooltip="Component" display="'Murata" xr:uid="{6EA63044-4ADE-4422-A47F-240ADA9440DE}"/>
+    <hyperlink ref="H20" r:id="rId56" tooltip="Manufacturer" display="'BLM18PG-121SN1D" xr:uid="{30EB9338-DDCA-4A35-8340-B3AC94FC63E7}"/>
+    <hyperlink ref="J20" r:id="rId57" tooltip="Supplier" display="'490-1037-1-ND" xr:uid="{4A15E6B9-3153-4A63-B4FA-1D2CF6CD443F}"/>
+    <hyperlink ref="G21" r:id="rId58" tooltip="Component" display="'Memory Protection Devices" xr:uid="{F6B43123-6130-4154-8C92-067F1D2334FD}"/>
+    <hyperlink ref="H21" r:id="rId59" tooltip="Manufacturer" display="'BK-6013" xr:uid="{0F87D72F-3728-4A37-BD56-976B7CEE0FC8}"/>
+    <hyperlink ref="J21" r:id="rId60" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{8AE79EEB-B78D-4A1F-89DC-6270737E8B77}"/>
+    <hyperlink ref="G22" tooltip="Component" display="'Generic Header" xr:uid="{2B78A5B2-7C50-4AB3-B09A-42D665E708C6}"/>
+    <hyperlink ref="H22" tooltip="Manufacturer" display="'" xr:uid="{48AE9638-161F-480A-A29F-8420D3562439}"/>
+    <hyperlink ref="J22" tooltip="Supplier" display="'" xr:uid="{664291A6-1D5D-446D-A2BE-9CD58E879A77}"/>
+    <hyperlink ref="G23" tooltip="Component" display="'Generic Header" xr:uid="{57A36B36-7469-41E9-8CC6-BA8564E84DC0}"/>
+    <hyperlink ref="H23" tooltip="Manufacturer" display="'" xr:uid="{B0B866B5-1C99-4694-81EF-EC75FC896D07}"/>
+    <hyperlink ref="J23" tooltip="Supplier" display="'" xr:uid="{B02FADAB-AB17-4890-BC75-C1B0EAA77031}"/>
+    <hyperlink ref="G24" tooltip="Component" display="'Generic Header" xr:uid="{C4491D4A-2209-4F1C-A9AC-51A39797FF3C}"/>
+    <hyperlink ref="H24" tooltip="Manufacturer" display="'" xr:uid="{A2FF2374-A79C-4F3E-959A-779B79B045A3}"/>
+    <hyperlink ref="J24" tooltip="Supplier" display="'" xr:uid="{EEE462B3-6F74-470D-B900-6EE9065A1AA1}"/>
+    <hyperlink ref="G25" tooltip="Component" display="'Generic Header" xr:uid="{521D8702-4747-4E80-8452-7C304BEE2733}"/>
+    <hyperlink ref="H25" tooltip="Manufacturer" display="'" xr:uid="{732EDE00-FFBA-45C1-A27B-7BB2D856F802}"/>
+    <hyperlink ref="J25" tooltip="Supplier" display="'" xr:uid="{2CF7D49E-6955-449F-92E2-503C27B67061}"/>
+    <hyperlink ref="G26" tooltip="Component" display="'Generic Header" xr:uid="{6591A477-D00D-48EE-A98B-1027B6D67988}"/>
+    <hyperlink ref="H26" tooltip="Manufacturer" display="'" xr:uid="{A4662579-EAC7-460A-87A4-BC7DE896A97E}"/>
+    <hyperlink ref="J26" tooltip="Supplier" display="'" xr:uid="{6C0ABF56-BFA9-49D7-9499-529D70729F7B}"/>
+    <hyperlink ref="G27" tooltip="Component" display="'Generic Header" xr:uid="{F337233D-2035-487E-A1D9-DCEA024F0D02}"/>
+    <hyperlink ref="H27" tooltip="Manufacturer" display="'" xr:uid="{A8577F0C-355A-44D6-9B7B-81460E9BD863}"/>
+    <hyperlink ref="J27" tooltip="Supplier" display="'" xr:uid="{3EC2EEFF-BE42-4F38-8D33-573F7245B95C}"/>
+    <hyperlink ref="G28" tooltip="Component" display="'Generic Header" xr:uid="{05D45BBE-02C6-4736-B6C6-87669D9867F5}"/>
+    <hyperlink ref="H28" tooltip="Manufacturer" display="'" xr:uid="{A09ECC7B-1240-4939-869A-DC04EC0AC0B2}"/>
+    <hyperlink ref="J28" tooltip="Supplier" display="'" xr:uid="{FBF3E804-8FAB-42FC-A8C1-6ED5594CBE3D}"/>
+    <hyperlink ref="G29" tooltip="Component" display="'Generic Header" xr:uid="{79313BCA-71A5-49DE-B520-F112A3CEB72A}"/>
+    <hyperlink ref="H29" tooltip="Manufacturer" display="'" xr:uid="{F5AF7133-92CE-43C9-AD47-9A56AAEE101C}"/>
+    <hyperlink ref="J29" tooltip="Supplier" display="'" xr:uid="{DF784B51-AC43-4AFA-8224-17B18FC2DF5B}"/>
+    <hyperlink ref="G30" r:id="rId61" tooltip="Component" display="'Bourns" xr:uid="{72476782-725B-4836-B30A-5F04B1E69765}"/>
+    <hyperlink ref="H30" r:id="rId62" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{49ED557E-E1E8-45AE-9A63-10B8447404F6}"/>
+    <hyperlink ref="J30" r:id="rId63" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{9440515A-5E4E-4D06-88F0-BA53D1451DC4}"/>
+    <hyperlink ref="G31" r:id="rId64" tooltip="Component" display="'Bourns" xr:uid="{D503BDB2-E5DC-4754-8625-9C964F926D83}"/>
+    <hyperlink ref="H31" r:id="rId65" tooltip="Manufacturer" display="'SRN6045TA-4R7M" xr:uid="{6A6A8E17-9C34-4B61-B206-CCA3E43C446D}"/>
+    <hyperlink ref="J31" r:id="rId66" tooltip="Supplier" display="'SRN6045TA-4R7MCT-ND" xr:uid="{4B8192E7-6A41-494D-9F96-D60483EF27A5}"/>
+    <hyperlink ref="G32" r:id="rId67" tooltip="Component" display="'Vishay Lite-On" xr:uid="{F6863E90-9630-4867-ACB3-4661BFB00327}"/>
+    <hyperlink ref="H32" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{C3C539EC-4A7C-4648-97FF-AA2C94956F94}"/>
+    <hyperlink ref="J32" r:id="rId69" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{18F7C41C-4279-4EE7-BABA-013A2E1B749F}"/>
+    <hyperlink ref="G33" r:id="rId70" tooltip="Component" display="'Vishay Lite-On" xr:uid="{6BABB0C8-CDDA-41BE-A40F-4EE50157E2B7}"/>
+    <hyperlink ref="H33" r:id="rId71" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{A026D94A-46C9-41D3-8806-92BFEDB4E95C}"/>
+    <hyperlink ref="J33" r:id="rId72" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{376CF738-804C-46C2-BF5C-D7C7D3DB02E0}"/>
+    <hyperlink ref="G34" r:id="rId73" tooltip="Component" display="'Molex" xr:uid="{2B948D03-2C66-44CE-A196-80D63E0743B1}"/>
+    <hyperlink ref="H34" r:id="rId74" tooltip="Manufacturer" display="'105017-0001" xr:uid="{8B0BE957-B084-4855-826E-85ED0F19E7A2}"/>
+    <hyperlink ref="J34" r:id="rId75" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{00E63B04-0447-40A7-A180-74028F2A475F}"/>
+    <hyperlink ref="G35" r:id="rId76" tooltip="Component" display="'Nexperia USA" xr:uid="{A3F6559B-1011-44BC-8D80-2DC68569E2E6}"/>
+    <hyperlink ref="H35" r:id="rId77" tooltip="Manufacturer" display="'BUK9Y14-40B,115" xr:uid="{D9C38CEB-4400-45AD-A210-FC1A90A4BC26}"/>
+    <hyperlink ref="J35" r:id="rId78" tooltip="Supplier" display="'1727-4940-1-ND" xr:uid="{0A5A3436-2BDC-48F8-8A6D-175AF02FDD35}"/>
+    <hyperlink ref="G36" r:id="rId79" tooltip="Component" display="'Vishay Siliconix" xr:uid="{9DE4B88C-50AC-425D-9B79-796A34EEC5C9}"/>
+    <hyperlink ref="H36" r:id="rId80" tooltip="Manufacturer" display="'SISS10DN-T1-GE3" xr:uid="{72B65CFB-1C80-4086-BFCD-30354AFD8C30}"/>
+    <hyperlink ref="J36" r:id="rId81" tooltip="Supplier" display="'SISS10DN-T1-GE3CT-ND" xr:uid="{DB7AEA15-7A51-4E9C-9080-A22567CE3F86}"/>
+    <hyperlink ref="G37" r:id="rId82" tooltip="Component" display="'Bel" xr:uid="{6A0A4FC0-4724-4582-BCB5-AC93C4BBEEC5}"/>
+    <hyperlink ref="H37" r:id="rId83" tooltip="Manufacturer" display="'0ZCM0020FF2G" xr:uid="{A6F37006-0842-4732-9612-6E863E700860}"/>
+    <hyperlink ref="J37" r:id="rId84" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{800402B5-ACAD-4BFB-B73F-A0A48AC23D7D}"/>
+    <hyperlink ref="G38" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{ED7C1F86-B632-4202-867F-0185CD293172}"/>
+    <hyperlink ref="H38" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{38D79B7C-BA85-43FB-B73F-D0969D25E493}"/>
+    <hyperlink ref="J38" r:id="rId87" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{F6E1C28E-0F49-440D-8A39-864BAE9F5F43}"/>
+    <hyperlink ref="G39" r:id="rId88" tooltip="Component" display="'Yageo" xr:uid="{74564CFB-A322-4424-99DC-FE6C9F07D6AE}"/>
+    <hyperlink ref="H39" r:id="rId89" tooltip="Manufacturer" display="'RC0603JR-072K2L" xr:uid="{D17FB144-0023-402F-89E5-96FF926E3B96}"/>
+    <hyperlink ref="J39" r:id="rId90" tooltip="Supplier" display="'311-2.2KGRCT-ND" xr:uid="{EB3E7303-E5EA-4C77-A5E1-9CCFE2D1C936}"/>
+    <hyperlink ref="G40" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{DA4CC817-4B78-4AFF-9949-B1B39A548A14}"/>
+    <hyperlink ref="H40" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{65B517F5-7A0F-4C02-B9CC-B085F4646ADE}"/>
+    <hyperlink ref="J40" r:id="rId93" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{BD9637C6-FB04-4E01-B720-0D9B15B5D7F4}"/>
+    <hyperlink ref="G41" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{2B33EBD6-A64E-49EF-A6DC-AFFE82FCA54D}"/>
+    <hyperlink ref="H41" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-0754K9L" xr:uid="{29EDFB39-0137-42AE-A6B7-008358C6EE8C}"/>
+    <hyperlink ref="J41" r:id="rId96" tooltip="Supplier" display="'311-54.9KHRCT-ND" xr:uid="{BA59BE21-D887-40B9-8044-309FE181F322}"/>
+    <hyperlink ref="G42" r:id="rId97" tooltip="Component" display="'Yageo Phycomp" xr:uid="{B8312566-FF7B-44EE-85AF-73BBE82AF68D}"/>
+    <hyperlink ref="H42" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{58D0A6F7-7DF5-4DFE-B8E4-FE4775F78C8B}"/>
+    <hyperlink ref="J42" r:id="rId99" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{0A518F3B-D982-48DE-B35C-EB435F8D2591}"/>
+    <hyperlink ref="G43" r:id="rId100" tooltip="Component" display="'Yageo" xr:uid="{4467C6D7-B5B3-48D0-8C3B-B236E109B74E}"/>
+    <hyperlink ref="H43" r:id="rId101" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{F98BD6EA-66B0-482C-9E91-AA0EF8CEC42C}"/>
+    <hyperlink ref="J43" r:id="rId102" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{606C7ED0-EB2D-4E1A-A349-64409F00CA86}"/>
+    <hyperlink ref="G44" r:id="rId103" tooltip="Component" display="'Yageo" xr:uid="{5FB05D9E-13DA-4CEA-9D36-F2F18422EA35}"/>
+    <hyperlink ref="H44" r:id="rId104" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{56E0540E-BA25-4C70-9327-D26D7CC13532}"/>
+    <hyperlink ref="J44" r:id="rId105" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{8633DFF8-BEA1-4AC4-A340-027A99A25BA9}"/>
+    <hyperlink ref="G45" r:id="rId106" tooltip="Component" display="'Yageo" xr:uid="{1E8539C1-3A21-4F1E-8CEE-A91BE3ED9390}"/>
+    <hyperlink ref="H45" r:id="rId107" tooltip="Manufacturer" display="'RC0603FR-07140KL" xr:uid="{A5E5035C-57C4-47B1-9FF2-696CCCD0D1D5}"/>
+    <hyperlink ref="J45" r:id="rId108" tooltip="Supplier" display="'311-140KHRCT-ND" xr:uid="{1356020A-E5C4-470C-896B-703A76126CB9}"/>
+    <hyperlink ref="G46" r:id="rId109" tooltip="Component" display="'Phoenix Contact" xr:uid="{CC8D370D-E3C9-410A-86AB-88288E980668}"/>
+    <hyperlink ref="H46" r:id="rId110" tooltip="Manufacturer" display="'MKDS1/4-3,5" xr:uid="{5FB04EC5-7046-4735-B597-879AA20E15D6}"/>
+    <hyperlink ref="J46" r:id="rId111" tooltip="Supplier" display="'277-5744-ND" xr:uid="{BDDCEC53-C31B-4279-A5B9-9F7A5C211FAF}"/>
+    <hyperlink ref="G47" r:id="rId112" tooltip="Component" display="'Phoenix Contact" xr:uid="{3D660BB5-C3B0-46A4-B81E-E59584B365B7}"/>
+    <hyperlink ref="H47" r:id="rId113" tooltip="Manufacturer" display="'MKDS1/2-3,5" xr:uid="{331DA305-4595-4621-BF04-5BDD58709C70}"/>
+    <hyperlink ref="J47" r:id="rId114" tooltip="Supplier" display="'277-5719-ND" xr:uid="{1511EE5A-9A3D-450A-8A7E-7CE2262BC6F9}"/>
+    <hyperlink ref="G48" r:id="rId115" tooltip="Component" display="'Phoenix Contact" xr:uid="{B59CDF0A-98CE-4150-A5D3-62B36FAC1B97}"/>
+    <hyperlink ref="H48" r:id="rId116" tooltip="Manufacturer" display="'1935776" xr:uid="{40103F51-3911-4920-9773-160B1B5AAEF1}"/>
+    <hyperlink ref="J48" r:id="rId117" tooltip="Supplier" display="'277-6405-ND" xr:uid="{ABEF7DEC-5151-4391-B788-31777631DD89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId115"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId118"/>
 </worksheet>
 </file>
</xml_diff>